<commit_message>
feat: Implement AI-powered PDF and CSV processing, analysis, and chat functionalities with Groq integration.
</commit_message>
<xml_diff>
--- a/exports/updated_data.xlsx
+++ b/exports/updated_data.xlsx
@@ -11,195 +11,174 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
-  <si>
-    <t>samagraFamilyId</t>
-  </si>
-  <si>
-    <t>headOfFamily_name</t>
-  </si>
-  <si>
-    <t>headOfFamily_address_houseNo</t>
-  </si>
-  <si>
-    <t>headOfFamily_address_street</t>
-  </si>
-  <si>
-    <t>headOfFamily_address_city</t>
-  </si>
-  <si>
-    <t>headOfFamily_address_pincode</t>
-  </si>
-  <si>
-    <t>headOfFamily_address_wardNo</t>
-  </si>
-  <si>
-    <t>headOfFamily_address_zone</t>
-  </si>
-  <si>
-    <t>headOfFamily_aadhaarAddress_houseNo</t>
-  </si>
-  <si>
-    <t>headOfFamily_aadhaarAddress_street</t>
-  </si>
-  <si>
-    <t>headOfFamily_aadhaarAddress_city</t>
-  </si>
-  <si>
-    <t>headOfFamily_aadhaarAddress_pincode</t>
-  </si>
-  <si>
-    <t>familyMembers_1_samagraId</t>
-  </si>
-  <si>
-    <t>familyMembers_1_name</t>
-  </si>
-  <si>
-    <t>familyMembers_1_age</t>
-  </si>
-  <si>
-    <t>familyMembers_1_gender</t>
-  </si>
-  <si>
-    <t>familyMembers_1_registrationDate</t>
-  </si>
-  <si>
-    <t>familyMembers_1_registeredBy</t>
-  </si>
-  <si>
-    <t>familyMembers_2_samagraId</t>
-  </si>
-  <si>
-    <t>familyMembers_2_name</t>
-  </si>
-  <si>
-    <t>familyMembers_2_age</t>
-  </si>
-  <si>
-    <t>familyMembers_2_gender</t>
-  </si>
-  <si>
-    <t>familyMembers_2_registrationDate</t>
-  </si>
-  <si>
-    <t>familyMembers_2_registeredBy</t>
-  </si>
-  <si>
-    <t>familyMembers_3_samagraId</t>
-  </si>
-  <si>
-    <t>familyMembers_3_name</t>
-  </si>
-  <si>
-    <t>familyMembers_3_age</t>
-  </si>
-  <si>
-    <t>familyMembers_3_gender</t>
-  </si>
-  <si>
-    <t>familyMembers_3_registrationDate</t>
-  </si>
-  <si>
-    <t>familyMembers_3_registeredBy</t>
-  </si>
-  <si>
-    <t>familyMembers_4_samagraId</t>
-  </si>
-  <si>
-    <t>familyMembers_4_name</t>
-  </si>
-  <si>
-    <t>familyMembers_4_age</t>
-  </si>
-  <si>
-    <t>familyMembers_4_gender</t>
-  </si>
-  <si>
-    <t>familyMembers_4_registrationDate</t>
-  </si>
-  <si>
-    <t>familyMembers_4_registeredBy</t>
-  </si>
-  <si>
-    <t>registrationDetails_registrationDate</t>
-  </si>
-  <si>
-    <t>registrationDetails_registeredBy</t>
-  </si>
-  <si>
-    <t>cardDetails_cardUpdateDate</t>
-  </si>
-  <si>
-    <t>cardDetails_ipAddress</t>
-  </si>
-  <si>
-    <t>**42883434**</t>
-  </si>
-  <si>
-    <t>Shekhar Jain</t>
-  </si>
-  <si>
-    <t>155, Ews 155/355</t>
-  </si>
-  <si>
-    <t>Indra Nagar Agar Road</t>
-  </si>
-  <si>
-    <t>Ujjain</t>
-  </si>
-  <si>
-    <t>456001</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>जोन 1</t>
-  </si>
-  <si>
-    <t>EWS-155/355</t>
-  </si>
-  <si>
-    <t>1192689160</t>
-  </si>
-  <si>
-    <t>पु.</t>
-  </si>
-  <si>
-    <t>01/09/2014</t>
-  </si>
-  <si>
-    <t>Sourabh</t>
-  </si>
-  <si>
-    <t>2192689210</t>
-  </si>
-  <si>
-    <t>Ranu Jain</t>
-  </si>
-  <si>
-    <t>म.</t>
-  </si>
-  <si>
-    <t>3192689246</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+  <si>
+    <t>reportName</t>
+  </si>
+  <si>
+    <t>generationDate</t>
+  </si>
+  <si>
+    <t>agentDetails_name</t>
+  </si>
+  <si>
+    <t>agentDetails_email</t>
+  </si>
+  <si>
+    <t>reportSummary_periodType</t>
+  </si>
+  <si>
+    <t>reportSummary_netQuantity</t>
+  </si>
+  <si>
+    <t>stockTransactions_1_date</t>
+  </si>
+  <si>
+    <t>stockTransactions_1_product</t>
+  </si>
+  <si>
+    <t>stockTransactions_1_txnId</t>
+  </si>
+  <si>
+    <t>stockTransactions_1_status</t>
+  </si>
+  <si>
+    <t>stockTransactions_1_quantity</t>
+  </si>
+  <si>
+    <t>stockTransactions_2_date</t>
+  </si>
+  <si>
+    <t>stockTransactions_2_product</t>
+  </si>
+  <si>
+    <t>stockTransactions_2_txnId</t>
+  </si>
+  <si>
+    <t>stockTransactions_2_status</t>
+  </si>
+  <si>
+    <t>stockTransactions_2_quantity</t>
+  </si>
+  <si>
+    <t>stockTransactions_3_date</t>
+  </si>
+  <si>
+    <t>stockTransactions_3_product</t>
+  </si>
+  <si>
+    <t>stockTransactions_3_txnId</t>
+  </si>
+  <si>
+    <t>stockTransactions_3_status</t>
+  </si>
+  <si>
+    <t>stockTransactions_3_quantity</t>
+  </si>
+  <si>
+    <t>stockTransactions_4_date</t>
+  </si>
+  <si>
+    <t>stockTransactions_4_product</t>
+  </si>
+  <si>
+    <t>stockTransactions_4_txnId</t>
+  </si>
+  <si>
+    <t>stockTransactions_4_status</t>
+  </si>
+  <si>
+    <t>stockTransactions_4_quantity</t>
+  </si>
+  <si>
+    <t>stockTransactions_5_date</t>
+  </si>
+  <si>
+    <t>stockTransactions_5_product</t>
+  </si>
+  <si>
+    <t>stockTransactions_5_txnId</t>
+  </si>
+  <si>
+    <t>stockTransactions_5_status</t>
+  </si>
+  <si>
+    <t>stockTransactions_5_quantity</t>
+  </si>
+  <si>
+    <t>stockTransactions_6_date</t>
+  </si>
+  <si>
+    <t>stockTransactions_6_product</t>
+  </si>
+  <si>
+    <t>stockTransactions_6_txnId</t>
+  </si>
+  <si>
+    <t>stockTransactions_6_status</t>
+  </si>
+  <si>
+    <t>stockTransactions_6_quantity</t>
+  </si>
+  <si>
+    <t>stockSummary_stockIn</t>
+  </si>
+  <si>
+    <t>stockSummary_stockOut</t>
+  </si>
+  <si>
+    <t>stockSummary_netChange</t>
+  </si>
+  <si>
+    <t>Stock Report</t>
+  </si>
+  <si>
+    <t>2/10/2026 12:13:25 PM</t>
   </si>
   <si>
     <t>Jatin Jain</t>
   </si>
   <si>
-    <t>4192689285</t>
-  </si>
-  <si>
-    <t>Jiya Jain</t>
-  </si>
-  <si>
-    <t>01/09/2014 6:11:00 PM</t>
-  </si>
-  <si>
-    <t>12/07/2025 1:45:57 PM</t>
-  </si>
-  <si>
-    <t>10.115.246.14</t>
+    <t>jjain0740@gmail.com</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Feb 9, 2026</t>
+  </si>
+  <si>
+    <t>Mini DryTab Lime Automatic Toilet Bowl Cleaner-Freshener</t>
+  </si>
+  <si>
+    <t>OUTSTK_64111</t>
+  </si>
+  <si>
+    <t>APPROVED</t>
+  </si>
+  <si>
+    <t>INSTK_35310</t>
+  </si>
+  <si>
+    <t>REJECTED</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Feb 4, 2026</t>
+  </si>
+  <si>
+    <t>I may disagree with what you say, but I will defend to death your right to say it. (Evelyn Beatrice Hall)</t>
+  </si>
+  <si>
+    <t>OUTSTK_11109</t>
+  </si>
+  <si>
+    <t>Laptop 1</t>
+  </si>
+  <si>
+    <t>nackband</t>
   </si>
 </sst>
 </file>
@@ -580,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN2"/>
+  <dimension ref="A1:AM2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,130 +680,124 @@
       <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2">
+        <v>-3</v>
+      </c>
+      <c r="G2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>46</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>47</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2">
+        <v>-1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
         <v>48</v>
       </c>
-      <c r="J2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
+        <v>49</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>44</v>
       </c>
-      <c r="L2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" t="s">
         <v>49</v>
       </c>
-      <c r="N2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2">
-        <v>49</v>
-      </c>
-      <c r="P2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
         <v>51</v>
       </c>
-      <c r="R2" t="s">
+      <c r="W2" t="s">
         <v>52</v>
       </c>
-      <c r="S2" t="s">
+      <c r="X2" t="s">
         <v>53</v>
       </c>
-      <c r="T2" t="s">
+      <c r="Y2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2">
+        <v>-1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" t="s">
         <v>54</v>
       </c>
-      <c r="U2">
-        <v>43</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="AC2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE2">
+        <v>-1</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2" t="s">
         <v>55</v>
       </c>
-      <c r="W2" t="s">
-        <v>51</v>
-      </c>
-      <c r="X2" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA2">
-        <v>21</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG2">
-        <v>17</v>
-      </c>
       <c r="AH2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AI2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>62</v>
+        <v>47</v>
+      </c>
+      <c r="AJ2">
+        <v>-2</v>
+      </c>
+      <c r="AK2">
+        <v>2</v>
+      </c>
+      <c r="AL2">
+        <v>-5</v>
+      </c>
+      <c r="AM2">
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>